<commit_message>
Changes: * Adjusted Readme.md file with example on how to debug using several key presses   with Virtual Piano Keyboard * Added Keyboard map for working with bass-pedal-config*.xml examples
</commit_message>
<xml_diff>
--- a/assets/midi_note_reference.xlsx
+++ b/assets/midi_note_reference.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Private\Audio&amp;Music\Behringer\Bass Pedal\Raspbery Pi\JMMidiBassPedalController\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Private\Audio&amp;Music\Behringer\Bass Pedal\Raspbery Pi\JMMidiBassPedalController\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8623"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Octave</t>
   </si>
@@ -133,6 +133,45 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Keys for Virtual Piano Keyboard Map</t>
   </si>
 </sst>
 </file>
@@ -169,15 +208,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor theme="0" tint="-0.34998626667073579"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,11 +236,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,9 +317,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -302,7 +436,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -564,26 +698,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="13" width="6.140625" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" customWidth="1"/>
-    <col min="16" max="18" width="7.5703125" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" customWidth="1"/>
-    <col min="21" max="32" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.15234375" customWidth="1"/>
+    <col min="2" max="13" width="6.15234375" customWidth="1"/>
+    <col min="15" max="15" width="21.3046875" customWidth="1"/>
+    <col min="16" max="18" width="7.53515625" customWidth="1"/>
+    <col min="19" max="20" width="9.69140625" customWidth="1"/>
+    <col min="21" max="32" width="4.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <f>FIRST_OCTAVE</f>
         <v>-2</v>
@@ -765,7 +899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>-1</v>
@@ -832,7 +966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A12" si="12">A3+1</f>
         <v>0</v>
@@ -893,7 +1027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <f t="shared" si="12"/>
         <v>1</v>
@@ -954,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <f t="shared" si="12"/>
         <v>2</v>
@@ -1008,7 +1142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <f t="shared" si="12"/>
         <v>3</v>
@@ -1062,7 +1196,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <f t="shared" si="12"/>
         <v>4</v>
@@ -1116,7 +1250,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <f t="shared" si="12"/>
         <v>5</v>
@@ -1170,7 +1304,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <f t="shared" si="12"/>
         <v>6</v>
@@ -1224,7 +1358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <f t="shared" si="12"/>
         <v>7</v>
@@ -1278,7 +1412,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <f t="shared" si="12"/>
         <v>8</v>
@@ -1328,10 +1462,126 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="B14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A16" s="8">
+        <v>2</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B14:M14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>